<commit_message>
feat: V3 mety mba handeha ngamba
</commit_message>
<xml_diff>
--- a/todo-list/suivi-todolist.xlsx
+++ b/todo-list/suivi-todolist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Recap" sheetId="1" state="visible" r:id="rId3"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="74">
   <si>
     <t xml:space="preserve">Avancement</t>
   </si>
@@ -79,55 +79,154 @@
     <t xml:space="preserve">Status</t>
   </si>
   <si>
+    <t xml:space="preserve">Base de donnee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MYSQL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">202602164014-1-base.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Création de la base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAMY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK</t>
+  </si>
+  <si>
     <t xml:space="preserve">Web</t>
   </si>
   <si>
-    <t xml:space="preserve">Login</t>
-  </si>
-  <si>
-    <t xml:space="preserve">index.php</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Création html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Affichage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Design css</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fonctions.php</t>
-  </si>
-  <si>
-    <t xml:space="preserve">checkLogin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fonction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">table login</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Base</t>
-  </si>
-  <si>
-    <t xml:space="preserve">données test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">traitement-login.php</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fonctionnement login</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Code intégration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mobile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dashboard</t>
+    <t xml:space="preserve">FLIGHT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">config.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initialisation de config</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOAVINA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initialisation de model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITOKIANA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VilleController.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fonctions CRUD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">controller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BesoinController.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saisie de besoin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dashboard.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tableau couverture par ville</t>
+  </si>
+  <si>
+    <t xml:space="preserve">view</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEPASSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DonController.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saisie des dons + donateurs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ville.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formulaire + liste des villes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">besoin.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formulaire + qte restante</t>
+  </si>
+  <si>
+    <t xml:space="preserve">don.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formulaire donateur+don+liste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dispatch.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bouton simulation + historique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">view/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verfication + quelques integrations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">style.css</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Style</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initialisation des nouveaux models</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RecapController.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">recapitulation besoin et don</t>
+  </si>
+  <si>
+    <t xml:space="preserve">recapitulation.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Affichage des recap besoin et don</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AchatController.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuration des frais d’achat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">achat.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Historique des achats + dons argents dispo</t>
   </si>
   <si>
     <t xml:space="preserve">estimation total</t>
@@ -334,7 +433,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
@@ -342,54 +441,58 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -397,35 +500,35 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -437,12 +540,12 @@
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Coin de la table dynamique" xfId="20"/>
-    <cellStyle name="Valeur de la table dynamique" xfId="21"/>
-    <cellStyle name="Champ de la table dynamique" xfId="22"/>
-    <cellStyle name="Catégorie de la table dynamique" xfId="23"/>
+    <cellStyle name="Catégorie de la table dynamique" xfId="20"/>
+    <cellStyle name="Champ de la table dynamique" xfId="21"/>
+    <cellStyle name="Coin de la table dynamique" xfId="22"/>
+    <cellStyle name="Résultat de la table dynamique" xfId="23"/>
     <cellStyle name="Titre de la table dynamique" xfId="24"/>
-    <cellStyle name="Résultat de la table dynamique" xfId="25"/>
+    <cellStyle name="Valeur de la table dynamique" xfId="25"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -508,88 +611,128 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" recordCount="7" createdVersion="3">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" recordCount="19" createdVersion="3">
   <cacheSource type="worksheet">
     <worksheetSource ref="C1:L20" sheet="liste des taches"/>
   </cacheSource>
   <cacheFields count="10">
     <cacheField name="Module" numFmtId="0">
-      <sharedItems containsBlank="1" count="3">
-        <s v="dashboard"/>
-        <s v="Login"/>
-        <m/>
+      <sharedItems count="2">
+        <s v="FLIGHT"/>
+        <s v="MYSQL"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Nom page" numFmtId="0">
-      <sharedItems containsBlank="1" count="4">
-        <s v="fonctions.php"/>
-        <s v="index.php"/>
-        <s v="traitement-login.php"/>
+      <sharedItems containsBlank="1" count="18">
+        <s v="202602164014-1-base.sql"/>
+        <s v="achat.php"/>
+        <s v="AchatController.php"/>
+        <s v="besoin.php"/>
+        <s v="BesoinController.php"/>
+        <s v="config.php"/>
+        <s v="Dashboard.php"/>
+        <s v="dispatch.php"/>
+        <s v="don.php"/>
+        <s v="DonController.php"/>
+        <s v="model/"/>
+        <s v="RecapController.php"/>
+        <s v="recapitulation.php"/>
+        <s v="style.css"/>
+        <s v="view/"/>
+        <s v="ville.php"/>
+        <s v="VilleController.php"/>
         <m/>
       </sharedItems>
     </cacheField>
     <cacheField name="Description" numFmtId="0">
-      <sharedItems containsBlank="1" count="7">
-        <s v="checkLogin"/>
-        <s v="Création html"/>
-        <s v="Design css"/>
-        <s v="données test"/>
-        <s v="fonctionnement login"/>
-        <s v="table login"/>
+      <sharedItems containsBlank="1" count="19">
+        <s v=" tableau couverture par ville"/>
+        <s v="Affichage des recap besoin et don"/>
+        <s v="Bouton simulation + historique"/>
+        <s v="Configuration des frais d’achat"/>
+        <s v="Création de la base"/>
+        <s v="Fonctions CRUD"/>
+        <s v="Formulaire + liste des villes "/>
+        <s v="Formulaire + qte restante"/>
+        <s v="Formulaire donateur+don+liste"/>
+        <s v="Historique des achats + dons argents dispo"/>
+        <s v="Initialisation de config"/>
+        <s v="Initialisation de model"/>
+        <s v="Initialisation des nouveaux models"/>
+        <s v="recapitulation besoin et don"/>
+        <s v="Saisie de besoin"/>
+        <s v="Saisie des dons + donateurs"/>
+        <s v="Style"/>
+        <s v="Verfication + quelques integrations"/>
         <m/>
       </sharedItems>
     </cacheField>
     <cacheField name="Type" numFmtId="0">
-      <sharedItems containsBlank="1" count="5">
-        <s v="Affichage"/>
-        <s v="Base"/>
-        <s v="Code intégration"/>
-        <s v="Fonction"/>
+      <sharedItems containsBlank="1" count="7">
+        <s v="Base de donnee"/>
+        <s v="controller"/>
+        <s v="Design"/>
+        <s v="Integration"/>
+        <s v="model"/>
+        <s v="view"/>
         <m/>
       </sharedItems>
     </cacheField>
     <cacheField name="Estimation" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="10" maxValue="180" count="5">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="10" maxValue="60" count="7">
         <n v="10"/>
         <n v="15"/>
+        <n v="20"/>
         <n v="30"/>
-        <n v="180"/>
+        <n v="40"/>
+        <n v="60"/>
         <m/>
       </sharedItems>
     </cacheField>
     <cacheField name="Temps passé" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="20" count="4">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="4" maxValue="60" count="8">
+        <n v="4"/>
+        <n v="5"/>
+        <n v="10"/>
+        <n v="15"/>
+        <n v="20"/>
+        <n v="40"/>
+        <n v="60"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Reste à faire" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="-5" maxValue="20" count="6">
+        <n v="-5"/>
         <n v="0"/>
-        <n v="10"/>
+        <n v="5"/>
+        <n v="16"/>
         <n v="20"/>
         <m/>
       </sharedItems>
     </cacheField>
-    <cacheField name="Reste à faire" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="5" maxValue="180" count="5">
-        <n v="5"/>
-        <n v="10"/>
-        <n v="30"/>
-        <n v="180"/>
-        <m/>
-      </sharedItems>
-    </cacheField>
     <cacheField name="Avancement" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0" maxValue="0.666666666666667" count="3">
-        <n v="0"/>
-        <n v="0.666666666666667"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.2" maxValue="1.5" count="6">
+        <n v="0.2"/>
+        <n v="0.333333333333333"/>
+        <n v="0.5"/>
+        <n v="1"/>
+        <n v="1.5"/>
         <m/>
       </sharedItems>
     </cacheField>
     <cacheField name="Qui" numFmtId="0">
-      <sharedItems containsBlank="1" count="3">
-        <s v="RAKOTO"/>
-        <s v="RASOA"/>
+      <sharedItems containsBlank="1" count="4">
+        <s v="ITOKIANA"/>
+        <s v="MAMY"/>
+        <s v="TOAVINA"/>
         <m/>
       </sharedItems>
     </cacheField>
     <cacheField name="Status" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" count="1">
+      <sharedItems containsBlank="1" count="3">
+        <s v="DEPASSE"/>
+        <s v="OK"/>
         <m/>
       </sharedItems>
     </cacheField>
@@ -598,97 +741,241 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="7">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="19">
   <r>
     <x v="1"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="3"/>
     <x v="1"/>
     <x v="1"/>
+  </r>
+  <r>
     <x v="0"/>
+    <x v="5"/>
+    <x v="10"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="10"/>
+    <x v="11"/>
+    <x v="4"/>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="16"/>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="14"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="6"/>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="9"/>
+    <x v="15"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="15"/>
+    <x v="6"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="1"/>
     <x v="2"/>
     <x v="2"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="3"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="5"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="3"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="4"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
   </r>
   <r>
     <x v="0"/>
     <x v="3"/>
-    <x v="6"/>
+    <x v="7"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="8"/>
+    <x v="8"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="7"/>
+    <x v="2"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="14"/>
+    <x v="17"/>
+    <x v="3"/>
+    <x v="2"/>
     <x v="4"/>
+    <x v="1"/>
     <x v="3"/>
     <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="13"/>
+    <x v="16"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="1"/>
     <x v="3"/>
     <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
     <x v="0"/>
+    <x v="10"/>
+    <x v="12"/>
+    <x v="4"/>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="1"/>
+    <x v="3"/>
     <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="11"/>
+    <x v="13"/>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="6"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="12"/>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="9"/>
+    <x v="5"/>
+    <x v="4"/>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="17"/>
+    <x v="18"/>
+    <x v="6"/>
+    <x v="6"/>
+    <x v="7"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="3"/>
+    <x v="2"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Recap" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" showDrill="1" useAutoFormatting="0" itemPrintTitles="1" indent="0" outline="0" outlineData="0" compact="0" compactData="0">
-  <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <location ref="A3:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField compact="0" showAll="0" outline="0"/>
     <pivotField compact="0" showAll="0" outline="0"/>
@@ -699,7 +986,8 @@
     <pivotField compact="0" showAll="0" outline="0"/>
     <pivotField compact="0" showAll="0" outline="0"/>
     <pivotField axis="axisRow" compact="0" showAll="0" outline="0">
-      <items count="4">
+      <items count="5">
+        <item x="3"/>
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -837,56 +1125,56 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="0" width="10.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="1" width="10.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="n">
+      <c r="B1" s="3" t="n">
         <f aca="false">'avancement projet'!D2</f>
-        <v>0.09836065574</v>
+        <v>0.894117647058824</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="n">
+      <c r="B4" s="7" t="n">
         <v>270</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="n">
+      <c r="B5" s="9" t="n">
         <v>35</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="9"/>
+      <c r="B6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="11" t="n">
+      <c r="B7" s="12" t="n">
         <v>305</v>
       </c>
     </row>
@@ -1901,342 +2189,914 @@
   </sheetPr>
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G41" activeCellId="0" sqref="G41"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="0" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="12" style="0" width="10.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="36.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="1" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="12.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="12" style="1" width="10.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14" t="n">
+      <c r="A2" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="16" t="n">
+        <v>10</v>
+      </c>
+      <c r="H2" s="16" t="n">
+        <v>10</v>
+      </c>
+      <c r="I2" s="16" t="n">
+        <f aca="false">G2-H2</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="17" t="n">
+        <f aca="false">(H2/(H2+I2))</f>
+        <v>1</v>
+      </c>
+      <c r="K2" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="15" t="n">
-        <v>30</v>
-      </c>
-      <c r="H2" s="15" t="n">
-        <f aca="false">detail!B2</f>
-        <v>20</v>
-      </c>
-      <c r="I2" s="15" t="n">
-        <f aca="false">G2-H2</f>
-        <v>10</v>
-      </c>
-      <c r="J2" s="16" t="n">
-        <f aca="false">(H2/(H2+I2))</f>
-        <v>0.666666666666667</v>
-      </c>
-      <c r="K2" s="15" t="s">
-        <v>3</v>
+      <c r="L2" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="14" t="n">
+      <c r="A3" s="15" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="15" t="s">
+      <c r="G3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="I3" s="16" t="n">
+        <f aca="false">G3-H3</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="17" t="n">
+        <f aca="false">(H3/(H3+I3))</f>
+        <v>1</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="15" t="n">
-        <v>30</v>
-      </c>
-      <c r="H3" s="15" t="n">
-        <f aca="false">detail!B3</f>
-        <v>0</v>
-      </c>
-      <c r="I3" s="15" t="n">
-        <f aca="false">G3-H3</f>
-        <v>30</v>
-      </c>
-      <c r="J3" s="16" t="n">
-        <f aca="false">(H3/(H3+I3))</f>
-        <v>0</v>
-      </c>
-      <c r="K3" s="15" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="14" t="n">
+      <c r="A4" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="15" t="s">
+      <c r="B4" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="C4" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="15" t="n">
-        <v>15</v>
-      </c>
-      <c r="H4" s="15" t="n">
-        <f aca="false">detail!B4</f>
+      <c r="D4" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="H4" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="I4" s="15" t="n">
+      <c r="I4" s="16" t="n">
         <f aca="false">G4-H4</f>
-        <v>5</v>
-      </c>
-      <c r="J4" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="J4" s="17" t="n">
         <f aca="false">(H4/(H4+I4))</f>
-        <v>0.666666666666667</v>
-      </c>
-      <c r="K4" s="15" t="s">
-        <v>4</v>
+        <v>0.333333333333333</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14" t="n">
+      <c r="A5" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="15" t="s">
+      <c r="B5" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="I5" s="16" t="n">
+        <f aca="false">G5-H5</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="17" t="n">
+        <f aca="false">(H5/(H5+I5))</f>
+        <v>1</v>
+      </c>
+      <c r="K5" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="15" t="n">
-        <v>10</v>
-      </c>
-      <c r="H5" s="15" t="n">
-        <f aca="false">detail!B5</f>
-        <v>0</v>
-      </c>
-      <c r="I5" s="15" t="n">
-        <f aca="false">G5-H5</f>
-        <v>10</v>
-      </c>
-      <c r="J5" s="16" t="n">
-        <f aca="false">(H5/(H5+I5))</f>
-        <v>0</v>
-      </c>
-      <c r="K5" s="15" t="s">
-        <v>4</v>
+      <c r="L5" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="14" t="n">
+      <c r="A6" s="15" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="15" t="s">
+      <c r="B6" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="I6" s="16" t="n">
+        <f aca="false">G6-H6</f>
+        <v>16</v>
+      </c>
+      <c r="J6" s="17" t="n">
+        <f aca="false">(H6/(H6+I6))</f>
+        <v>0.2</v>
+      </c>
+      <c r="K6" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="15" t="n">
-        <v>10</v>
-      </c>
-      <c r="H6" s="15" t="n">
-        <f aca="false">detail!B6</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="15" t="n">
-        <f aca="false">G6-H6</f>
-        <v>10</v>
-      </c>
-      <c r="J6" s="16" t="n">
-        <f aca="false">(H6/(H6+I6))</f>
-        <v>0</v>
-      </c>
-      <c r="K6" s="15" t="s">
-        <v>4</v>
+      <c r="L6" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14" t="n">
+      <c r="A7" s="15" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="15" t="n">
-        <v>30</v>
-      </c>
-      <c r="H7" s="15" t="n">
-        <f aca="false">detail!B7</f>
-        <v>0</v>
-      </c>
-      <c r="I7" s="15" t="n">
+      <c r="B7" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="I7" s="16" t="n">
         <f aca="false">G7-H7</f>
-        <v>30</v>
-      </c>
-      <c r="J7" s="16" t="n">
+        <v>-5</v>
+      </c>
+      <c r="J7" s="17" t="n">
         <f aca="false">(H7/(H7+I7))</f>
-        <v>0</v>
-      </c>
-      <c r="K7" s="15" t="s">
-        <v>3</v>
+        <v>1.5</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14" t="n">
+      <c r="A8" s="15" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="15" t="n">
-        <v>180</v>
-      </c>
-      <c r="H8" s="15" t="n">
-        <f aca="false">detail!B8</f>
+      <c r="B8" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="I8" s="16" t="n">
+        <f aca="false">G8-H8</f>
         <v>0</v>
       </c>
-      <c r="I8" s="15" t="n">
-        <f aca="false">G8-H8</f>
-        <v>180</v>
-      </c>
-      <c r="J8" s="16" t="n">
+      <c r="J8" s="17" t="n">
         <f aca="false">(H8/(H8+I8))</f>
+        <v>1</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="15" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="H9" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="I9" s="16" t="n">
+        <f aca="false">G9-H9</f>
+        <v>5</v>
+      </c>
+      <c r="J9" s="17" t="n">
+        <f aca="false">(H9/(H9+I9))</f>
+        <v>0.5</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="15" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="H10" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="I10" s="16" t="n">
+        <f aca="false">G10-H10</f>
         <v>0</v>
       </c>
-      <c r="K8" s="15" t="s">
-        <v>3</v>
+      <c r="J10" s="17" t="n">
+        <f aca="false">(H10/(H10+I10))</f>
+        <v>1</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="15" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="I11" s="16" t="n">
+        <f aca="false">G11-H11</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="17" t="n">
+        <f aca="false">(H11/(H11+I11))</f>
+        <v>1</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="15" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="H12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="I12" s="16" t="n">
+        <f aca="false">G12-H12</f>
+        <v>0</v>
+      </c>
+      <c r="J12" s="17" t="n">
+        <f aca="false">(H12/(H12+I12))</f>
+        <v>1</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="15" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H13" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="I13" s="16" t="n">
+        <f aca="false">G13-H13</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="17" t="n">
+        <f aca="false">(H13/(H13+I13))</f>
+        <v>1</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="15" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="H14" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="I14" s="16" t="n">
+        <f aca="false">G14-H14</f>
+        <v>0</v>
+      </c>
+      <c r="J14" s="17" t="n">
+        <f aca="false">(H14/(H14+I14))</f>
+        <v>1</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H15" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="I15" s="16" t="n">
+        <f aca="false">G15-H15</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="17" t="n">
+        <f aca="false">(H15/(H15+I15))</f>
+        <v>1</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="15" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="H16" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="I16" s="16" t="n">
+        <f aca="false">G16-H16</f>
+        <v>0</v>
+      </c>
+      <c r="J16" s="17" t="n">
+        <f aca="false">(H16/(H16+I16))</f>
+        <v>1</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="15" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H17" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="I17" s="16" t="n">
+        <f aca="false">G17-H17</f>
+        <v>0</v>
+      </c>
+      <c r="J17" s="17" t="n">
+        <f aca="false">(H17/(H17+I17))</f>
+        <v>1</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="15" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H18" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="I18" s="16" t="n">
+        <f aca="false">G18-H18</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="17" t="n">
+        <f aca="false">(H18/(H18+I18))</f>
+        <v>1</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="15" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="H19" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="I19" s="16" t="n">
+        <f aca="false">G19-H19</f>
+        <v>0</v>
+      </c>
+      <c r="J19" s="17" t="n">
+        <f aca="false">(H19/(H19+I19))</f>
+        <v>1</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="15" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="15" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="15" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="15" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="15" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="15" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="15" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="15" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="15" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="15" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="15" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3224,66 +4084,66 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="6" style="0" width="10.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="6" style="1" width="10.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>38</v>
+      <c r="A1" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="n">
+      <c r="A2" s="16" t="n">
         <f aca="false">SUM('liste des taches'!G2:G329)</f>
-        <v>305</v>
-      </c>
-      <c r="B2" s="15" t="n">
+        <v>340</v>
+      </c>
+      <c r="B2" s="16" t="n">
         <f aca="false">SUM('liste des taches'!H2:H329)</f>
-        <v>30</v>
-      </c>
-      <c r="C2" s="15" t="n">
+        <v>304</v>
+      </c>
+      <c r="C2" s="16" t="n">
         <f aca="false">SUM('liste des taches'!I2:I329)</f>
-        <v>275</v>
-      </c>
-      <c r="D2" s="16" t="n">
+        <v>36</v>
+      </c>
+      <c r="D2" s="17" t="n">
         <f aca="false">(B2/(B2+C2))</f>
-        <v>0.09836065574</v>
-      </c>
-      <c r="E2" s="17" t="n">
+        <v>0.894117647058824</v>
+      </c>
+      <c r="E2" s="18" t="n">
         <f aca="false">((B2+C2)-A2)/A2</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C3" s="15" t="n">
+      <c r="C3" s="16" t="n">
         <f aca="false">C2/60</f>
-        <v>4.583333333</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>39</v>
+        <v>0.6</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -4307,95 +5167,95 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="1" style="0" width="10.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="1" style="1" width="10.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="18" t="n">
+      <c r="B1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="19" t="n">
         <v>46048</v>
       </c>
-      <c r="D1" s="18" t="n">
+      <c r="D1" s="19" t="n">
         <v>46049</v>
       </c>
-      <c r="E1" s="18" t="n">
+      <c r="E1" s="19" t="n">
         <v>46050</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14" t="n">
+      <c r="A2" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="n">
+      <c r="B2" s="16" t="n">
         <f aca="false">SUM(D2:P2)</f>
         <v>20</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14" t="n">
+      <c r="C2" s="15"/>
+      <c r="D2" s="15" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="14" t="n">
+      <c r="A3" s="15" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="15" t="n">
+      <c r="B3" s="16" t="n">
         <f aca="false">SUM(D3:P3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="14" t="n">
+      <c r="A4" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="15" t="n">
+      <c r="B4" s="16" t="n">
         <f aca="false">SUM(D4:P4)</f>
         <v>10</v>
       </c>
-      <c r="C4" s="14" t="n">
+      <c r="C4" s="15" t="n">
         <v>20</v>
       </c>
-      <c r="D4" s="14" t="n">
+      <c r="D4" s="15" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14" t="n">
+      <c r="A5" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="15" t="n">
+      <c r="B5" s="16" t="n">
         <f aca="false">SUM(D5:P5)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="14" t="n">
+      <c r="A6" s="15" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="15" t="n">
+      <c r="B6" s="16" t="n">
         <f aca="false">SUM(D6:P6)</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14" t="n">
+      <c r="A7" s="15" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="15" t="n">
+      <c r="B7" s="16" t="n">
         <f aca="false">SUM(D7:P7)</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14" t="n">
+      <c r="A8" s="15" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="15" t="n">
+      <c r="B8" s="16" t="n">
         <f aca="false">SUM(D8:P8)</f>
         <v>0</v>
       </c>

</xml_diff>